<commit_message>
- Se realiza la carga masiva
</commit_message>
<xml_diff>
--- a/GLOCSE/Assets/Plantilla.xlsx
+++ b/GLOCSE/Assets/Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\river\OneDrive\Documentos\Github\Glocse\GLOCSE\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\river\Documents\Github\Glocse\GLOCSE\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED077336-BF05-43A4-A4DB-62421FDB9854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2FF9B9-12FC-4428-BBEB-BE61B7DC56F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +178,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -187,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -278,11 +284,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,7 +310,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -313,12 +331,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,187 +622,187 @@
   <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="24" width="8.88671875" customWidth="1"/>
-    <col min="25" max="25" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="24" width="8.85546875" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" customWidth="1"/>
     <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.88671875" hidden="1"/>
+    <col min="27" max="16384" width="8.85546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -794,7 +814,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -806,113 +826,113 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="12"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="T11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="U11" s="4" t="s">
+      <c r="U11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="V11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="W11" s="4" t="s">
+      <c r="W11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="X11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="Y11" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -941,7 +961,7 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -958,7 +978,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="O13" s="14"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -970,7 +990,7 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -999,7 +1019,7 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1028,7 +1048,7 @@
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1057,7 +1077,7 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1086,7 +1106,7 @@
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1115,7 +1135,7 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1144,7 +1164,7 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1193,7 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>